<commit_message>
correction of python code with new sources
</commit_message>
<xml_diff>
--- a/Sources.xlsx
+++ b/Sources.xlsx
@@ -8,17 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aym3r\Documents\Cours\203\TWAG\weekly_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83765961-0BFD-4FC0-BFEE-993450794C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8C4A56-B156-453D-9C99-42912074261C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -114,57 +121,9 @@
     <t>Italy 10</t>
   </si>
   <si>
-    <t>https://www.wsj.com/market-data/quotes/index/SPX</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/DJIA</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/UK/UKX</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/DX/DAX</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/FR/PX1</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/XX/XSTX/SX5E</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/CN/SHCOMP</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/JP/XTKS/NIK</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/XX/990100</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/XX/891800</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/index/VIX</t>
-  </si>
-  <si>
     <t>https://www.wsj.com/market-data/quotes/futures/UK/BRENT%20CRUDE</t>
   </si>
   <si>
-    <t>https://www.wsj.com/market-data/quotes/futures/GOLD</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/fx/EURUSD</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/fx/USDJPY</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/fx/GBPUSD</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/fx/USDCHF</t>
-  </si>
-  <si>
     <t>https://www.global-rates.com/interest-rates/eonia/eonia.aspx</t>
   </si>
   <si>
@@ -174,25 +133,73 @@
     <t>https://www.global-rates.com/interest-rates/euribor/euribor-interest-3-months.aspx</t>
   </si>
   <si>
-    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMUBMUSD10Y</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKDE-10Y</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKFR-10Y</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKJP-10Y</t>
-  </si>
-  <si>
-    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKIT-10Y</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
     <t>rate</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/SPX/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/DJIA/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/UK/UKX/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/DX/DAX/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/FR/PX1/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/XX/XSTX/SX5E/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/CN/SHCOMP/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/JP/XTKS/NIK/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/XX/990100/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/XX/891800/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/index/VIX/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/fx/EURUSD/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/fx/USDJPY/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/fx/GBPUSD/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/fx/USDCHF/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMUBMUSD10Y/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKDE-10Y/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKFR-10Y/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKJP-10Y/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/bond/BX/TMBMKIT-10Y/historical-prices</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/market-data/quotes/futures/GOLD/</t>
   </si>
 </sst>
 </file>
@@ -552,7 +559,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,13 +587,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4">
         <v>3700.65</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -594,13 +601,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4">
         <v>30223.89</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -608,13 +615,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4">
         <v>6571.88</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -622,13 +629,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4">
         <v>13726.74</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -636,13 +643,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4">
         <v>5588.96</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -650,13 +657,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4">
         <v>3564.39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -664,13 +671,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4">
         <v>3502.96</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,13 +685,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4">
         <v>27258.38</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,13 +699,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4">
         <v>2690.04</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -706,13 +713,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
         <v>1291.75</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -720,13 +727,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4">
         <v>26.97</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -734,13 +741,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4">
         <v>51.09</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,13 +755,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4">
         <v>1895.1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -762,13 +769,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C15" s="4">
         <v>1.2215</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -776,13 +783,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4">
         <v>103.24</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -790,13 +797,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4">
         <v>1.3673</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -804,13 +811,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C18" s="4">
         <v>0.88490000000000002</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -818,13 +825,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4">
-        <v>-4.81E-3</v>
+        <v>-0.48099999999999998</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -832,13 +839,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C20" s="4">
-        <v>2.3725E-3</v>
+        <v>0.23725000000000002</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -846,13 +853,13 @@
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C21" s="4">
-        <v>-5.4599999999999996E-3</v>
+        <v>-0.54599999999999993</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -860,13 +867,13 @@
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="4">
-        <v>9.1699999999999993E-3</v>
+        <v>0.91699999999999993</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -874,13 +881,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="4">
-        <v>-6.0499999999999998E-3</v>
+        <v>-0.60499999999999998</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -888,13 +895,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4">
-        <v>-3.65E-3</v>
+        <v>-0.36499999999999999</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -902,13 +909,13 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4">
-        <v>4.4999999999999999E-4</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -916,13 +923,13 @@
         <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="4">
-        <v>5.5099999999999995E-4</v>
+        <v>5.5099999999999996E-2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -931,28 +938,29 @@
     <hyperlink ref="B21" r:id="rId2" xr:uid="{76BAB3F7-A0E5-437E-8FC6-40CD12B889F6}"/>
     <hyperlink ref="B19" r:id="rId3" xr:uid="{9393D8DE-15C1-4B67-980E-4E56FB537678}"/>
     <hyperlink ref="B25" r:id="rId4" xr:uid="{008BB9B4-4A46-4E2D-86DC-BEE84B7F9A8B}"/>
-    <hyperlink ref="B26" r:id="rId5" xr:uid="{BEAC819A-431E-4151-92AE-6BBD433D461D}"/>
-    <hyperlink ref="B11" r:id="rId6" xr:uid="{56BC43F7-0962-4CCB-9196-75247B86256D}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{45DC85D7-7AAC-4628-BB5C-A353BE5375A3}"/>
-    <hyperlink ref="B16" r:id="rId8" xr:uid="{C84A222A-B3A8-4876-BD48-AF223D5DA274}"/>
-    <hyperlink ref="B17" r:id="rId9" xr:uid="{70F149B6-E342-4651-8293-0BE429FED14A}"/>
-    <hyperlink ref="B18" r:id="rId10" xr:uid="{9DAC9CFE-DEA0-4126-B77E-96380508F039}"/>
-    <hyperlink ref="B2" r:id="rId11" xr:uid="{FD4E24C6-8143-4CAF-84CB-C85A05244360}"/>
-    <hyperlink ref="B3" r:id="rId12" xr:uid="{227223B1-E779-43AC-9A46-5C0CCF5F7FBD}"/>
-    <hyperlink ref="B4" r:id="rId13" xr:uid="{D2168CC5-C332-4DAE-BD2D-CB23FC2B92C7}"/>
-    <hyperlink ref="B5" r:id="rId14" xr:uid="{1146C274-D3B6-4967-A006-8FF252F71845}"/>
-    <hyperlink ref="B6" r:id="rId15" xr:uid="{85B8CBC6-BF04-4DB2-A0ED-C86323A04E54}"/>
-    <hyperlink ref="B7" r:id="rId16" xr:uid="{AFCF11CE-6316-4E18-A6EC-110A5637E132}"/>
-    <hyperlink ref="B8" r:id="rId17" xr:uid="{98473E02-866F-4AD5-AF53-0C2B27A5481B}"/>
-    <hyperlink ref="B9" r:id="rId18" xr:uid="{7CC84154-1F8A-4D1C-8F29-80671A45444A}"/>
-    <hyperlink ref="B12" r:id="rId19" xr:uid="{7E58576F-1292-46EF-A102-8C438EF288E7}"/>
-    <hyperlink ref="B13" r:id="rId20" display="https://www.wsj.com/market-data/quotes/futures/UK/BRENT CRUDE" xr:uid="{A29D076D-4D7B-40EA-8B47-04B79E34604B}"/>
-    <hyperlink ref="B14" r:id="rId21" xr:uid="{15C5D25E-7263-44EA-936F-10DE137FFF31}"/>
-    <hyperlink ref="B15" r:id="rId22" xr:uid="{B015D545-4DDD-4D7F-9528-0B8B2F44936C}"/>
-    <hyperlink ref="B22" r:id="rId23" xr:uid="{C247C2AC-3EBB-499C-B774-7D4667614CFE}"/>
-    <hyperlink ref="B23" r:id="rId24" xr:uid="{130856FC-B610-4771-8E8B-4DEB3C78F9B4}"/>
-    <hyperlink ref="B24" r:id="rId25" xr:uid="{2BF84AAA-AFCB-4AD5-AE57-9CFF8A179975}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{56BC43F7-0962-4CCB-9196-75247B86256D}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{45DC85D7-7AAC-4628-BB5C-A353BE5375A3}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{C84A222A-B3A8-4876-BD48-AF223D5DA274}"/>
+    <hyperlink ref="B17" r:id="rId8" xr:uid="{70F149B6-E342-4651-8293-0BE429FED14A}"/>
+    <hyperlink ref="B18" r:id="rId9" xr:uid="{9DAC9CFE-DEA0-4126-B77E-96380508F039}"/>
+    <hyperlink ref="B2" r:id="rId10" xr:uid="{FD4E24C6-8143-4CAF-84CB-C85A05244360}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{227223B1-E779-43AC-9A46-5C0CCF5F7FBD}"/>
+    <hyperlink ref="B4" r:id="rId12" xr:uid="{D2168CC5-C332-4DAE-BD2D-CB23FC2B92C7}"/>
+    <hyperlink ref="B5" r:id="rId13" xr:uid="{1146C274-D3B6-4967-A006-8FF252F71845}"/>
+    <hyperlink ref="B6" r:id="rId14" xr:uid="{85B8CBC6-BF04-4DB2-A0ED-C86323A04E54}"/>
+    <hyperlink ref="B7" r:id="rId15" xr:uid="{AFCF11CE-6316-4E18-A6EC-110A5637E132}"/>
+    <hyperlink ref="B8" r:id="rId16" xr:uid="{98473E02-866F-4AD5-AF53-0C2B27A5481B}"/>
+    <hyperlink ref="B12" r:id="rId17" xr:uid="{7E58576F-1292-46EF-A102-8C438EF288E7}"/>
+    <hyperlink ref="B13" r:id="rId18" xr:uid="{A29D076D-4D7B-40EA-8B47-04B79E34604B}"/>
+    <hyperlink ref="B14" r:id="rId19" xr:uid="{15C5D25E-7263-44EA-936F-10DE137FFF31}"/>
+    <hyperlink ref="B15" r:id="rId20" xr:uid="{B015D545-4DDD-4D7F-9528-0B8B2F44936C}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{C247C2AC-3EBB-499C-B774-7D4667614CFE}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{130856FC-B610-4771-8E8B-4DEB3C78F9B4}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{2BF84AAA-AFCB-4AD5-AE57-9CFF8A179975}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{BEAC819A-431E-4151-92AE-6BBD433D461D}"/>
+    <hyperlink ref="B9" r:id="rId25" xr:uid="{7CC84154-1F8A-4D1C-8F29-80671A45444A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>